<commit_message>
Add new templates for evidencia_ns and evidencia_vok; update existing templates for improved navigation and data display
</commit_message>
<xml_diff>
--- a/semana/semana_completa_19.xlsx
+++ b/semana/semana_completa_19.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28906"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28908"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{350E0901-C9C0-4B85-AF25-844A3D49A8FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{158633E1-87D0-4890-94E5-A18C2D44542D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="1" r:id="rId1"/>
@@ -13,6 +13,8 @@
     <sheet name="Detalle_VOK" sheetId="3" r:id="rId3"/>
     <sheet name="Carta_cr" sheetId="4" r:id="rId4"/>
     <sheet name="Detalle_cr" sheetId="5" r:id="rId5"/>
+    <sheet name="Evidencia_vok" sheetId="6" r:id="rId6"/>
+    <sheet name="Evidencia_ns" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Resumen!$A$1:$I$1</definedName>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3797" uniqueCount="969">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4291" uniqueCount="1039">
   <si>
     <t>c</t>
   </si>
@@ -2945,13 +2947,223 @@
   </si>
   <si>
     <t>E-WOL-N0096</t>
+  </si>
+  <si>
+    <t>PLANTA</t>
+  </si>
+  <si>
+    <t>RUTAS</t>
+  </si>
+  <si>
+    <t>V MALOS</t>
+  </si>
+  <si>
+    <t>INI RUTA</t>
+  </si>
+  <si>
+    <t>FIN RUTA</t>
+  </si>
+  <si>
+    <t>Observacion</t>
+  </si>
+  <si>
+    <t>0 a 4 min</t>
+  </si>
+  <si>
+    <t>11 a 15 min</t>
+  </si>
+  <si>
+    <t>No empieza en p 1</t>
+  </si>
+  <si>
+    <t>16 a 20 min</t>
+  </si>
+  <si>
+    <t>5 a 10 min</t>
+  </si>
+  <si>
+    <t>mayor a 21</t>
+  </si>
+  <si>
+    <t>inicio 40 minutos tarde</t>
+  </si>
+  <si>
+    <t>Puntual</t>
+  </si>
+  <si>
+    <t>un viaje no registro la llegada ya que por trafico llega 55 minutos tarde</t>
+  </si>
+  <si>
+    <t>un viaje inicia punto 3, 38 minutos tardey llegando a planta 33 min</t>
+  </si>
+  <si>
+    <t>2 viajes inciando 30 minutos tarde</t>
+  </si>
+  <si>
+    <t>iniciado 30 min tarde saltando puntos en el recorrido y llegando 40 min</t>
+  </si>
+  <si>
+    <t>un viaje llega arriba de 20 min a planta</t>
+  </si>
+  <si>
+    <t>2 viajes inician en tiempo y 2 tarde , 3 viajes llegan 16 a 20 y un viaje llega 40 min tarde a planta</t>
+  </si>
+  <si>
+    <t>1 viaje inicia 6 minutos tarde</t>
+  </si>
+  <si>
+    <t>un solo viaje llega 17 minutos tarde, los otros 2 viajes mas de 30 minutos</t>
+  </si>
+  <si>
+    <t>un vijae llega 14 min tarde y los demas mas de 30 minutos</t>
+  </si>
+  <si>
+    <t>un solo viaje incia 40 minutos tarde , un viaje llega 22 min tarde y otro 44 miuntos tarde</t>
+  </si>
+  <si>
+    <t>un solo viaje llega 20 min tarde por trafico</t>
+  </si>
+  <si>
+    <t>2 viajes llegando 35 min tarde</t>
+  </si>
+  <si>
+    <t>No registra el tiempo de llegada real</t>
+  </si>
+  <si>
+    <t>llega a planta 6:15 am</t>
+  </si>
+  <si>
+    <t>inicia 35 min tarde</t>
+  </si>
+  <si>
+    <t>iniciando en punto 2</t>
+  </si>
+  <si>
+    <t>llegando 27 min tarde desviandose en el trayecto</t>
+  </si>
+  <si>
+    <t>iniciando en punto 2 y llega 3 minutos tarde</t>
+  </si>
+  <si>
+    <t>no registro la hora real de llega llegando 5 minutos tarde</t>
+  </si>
+  <si>
+    <t>a mediados del recorrido regresa al punto 1 llegando 24 min tarde</t>
+  </si>
+  <si>
+    <t>llegando a planta 26 min tarde</t>
+  </si>
+  <si>
+    <t>realiza 2 recorridos y llega tarde</t>
+  </si>
+  <si>
+    <t>llega a planta 7:19 am</t>
+  </si>
+  <si>
+    <t>4 viajes llegan 10 min tarde y 4 viajes llegan arriba de 21 min</t>
+  </si>
+  <si>
+    <t>3 viajes llegan un rango de 6 a 12 miuntos, 2 viajes llegan mas de 25 min</t>
+  </si>
+  <si>
+    <t>1 solo viaje inicia 19 min tarde, un solo viaje llega 16 min tarde</t>
+  </si>
+  <si>
+    <t>un viaje inicia 49 min tarde y el mismo viaje llega 34 min tarde</t>
+  </si>
+  <si>
+    <t>inicia 41 min tarde</t>
+  </si>
+  <si>
+    <t>llega a planta 30 min tarde</t>
+  </si>
+  <si>
+    <t>inicia 48 min tarde y llega 27 min tarde</t>
+  </si>
+  <si>
+    <t>inicia 36 min tarde y llega 27 min tarde</t>
+  </si>
+  <si>
+    <t>llega 24 min tarde</t>
+  </si>
+  <si>
+    <t>1 viaje llega 19 min, 1 viaje llega 24 min y 3 viajes llegan mas de 40 min</t>
+  </si>
+  <si>
+    <t>inicia 23 min tarde,</t>
+  </si>
+  <si>
+    <t>2 viajes incian puntuales y 2 viajes incian 15 minutos tarde</t>
+  </si>
+  <si>
+    <t>un viajes inicia punto 2 y no registra hora real llegando puntual</t>
+  </si>
+  <si>
+    <t>un viaje inicia 40 min tarde y llega tarde 50 min tarde</t>
+  </si>
+  <si>
+    <t>un viaje inicia 13 min tarde</t>
+  </si>
+  <si>
+    <t>llegando 22 min tarde</t>
+  </si>
+  <si>
+    <t>1 viajes llega 15 min tarde y 2 viajes mas de 30 min</t>
+  </si>
+  <si>
+    <t>inicianan mas de 25 a 30 min tarde</t>
+  </si>
+  <si>
+    <t>inicia 39 minutos tarde y un viaje inicia puntual,</t>
+  </si>
+  <si>
+    <t>inicia 38 min tarde</t>
+  </si>
+  <si>
+    <t>1 viaje llega 7 minutos , 1 viaje llega 17 min y 1 viaje llega 44 min tarde</t>
+  </si>
+  <si>
+    <t>1 viaje inica 20 min tarde</t>
+  </si>
+  <si>
+    <t>llega en tiempo a planta</t>
+  </si>
+  <si>
+    <t>inicia 42 min tarde por iniciar hacer otro recorrido, y llega 30 min tarde</t>
+  </si>
+  <si>
+    <t>inicia 25 min tarde</t>
+  </si>
+  <si>
+    <t>llega 30 miuntos tarde por realizar 2 recorridos</t>
+  </si>
+  <si>
+    <t>2 viajes inician en tiempo</t>
+  </si>
+  <si>
+    <t>3 viajes llegan a 17 min y 9 viajes llegan de 5 a 13 min tarde a planta</t>
+  </si>
+  <si>
+    <t>2 viajes llegan mas de 30 min tarde</t>
+  </si>
+  <si>
+    <t>1 viajes inicia 38 min tarde y 1 viaje inicia 18 min tarde, 4 viajes llegan mas de 30 a 44 min tarde</t>
+  </si>
+  <si>
+    <t>1 viaje llega 33 min tarde y 1 viaje llega 15 min tarde, los demas de 5 a 10 min</t>
+  </si>
+  <si>
+    <t>11 a 21 min</t>
+  </si>
+  <si>
+    <t>inicia 45 min tarde y llegando 30 min tarde</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3005,8 +3217,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="20">
+  <fills count="31">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3121,8 +3352,74 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB5E6A2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF7E36F"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF63BE7B"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFE082"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFED480"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFDBC7B"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFEC87E"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFB9975"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFA8D72"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF8696B"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -3154,11 +3451,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF46B1E1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -3205,6 +3526,21 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -35495,8 +35831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62FFAE9B-274F-4256-B476-354716661A12}">
   <dimension ref="A1:F426"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T18" sqref="T18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -44024,4 +44360,2110 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F28AF2A-BC79-4F8D-9025-3938796825AE}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{123B88C3-7251-47CF-A744-0BF7EF379447}">
+  <dimension ref="A1:F109"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:F109"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="6" max="6" width="72.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="32" t="s">
+        <v>969</v>
+      </c>
+      <c r="B1" s="33" t="s">
+        <v>970</v>
+      </c>
+      <c r="C1" s="34" t="s">
+        <v>971</v>
+      </c>
+      <c r="D1" s="35" t="s">
+        <v>972</v>
+      </c>
+      <c r="E1" s="35" t="s">
+        <v>973</v>
+      </c>
+      <c r="F1" s="35" t="s">
+        <v>974</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="37">
+        <v>1</v>
+      </c>
+      <c r="D2" s="35" t="s">
+        <v>975</v>
+      </c>
+      <c r="E2" s="35" t="s">
+        <v>976</v>
+      </c>
+      <c r="F2" s="38"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" s="37">
+        <v>1</v>
+      </c>
+      <c r="D3" s="35" t="s">
+        <v>977</v>
+      </c>
+      <c r="E3" s="35" t="s">
+        <v>978</v>
+      </c>
+      <c r="F3" s="38"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" s="37">
+        <v>1</v>
+      </c>
+      <c r="D4" s="35" t="s">
+        <v>978</v>
+      </c>
+      <c r="E4" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="F4" s="38"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="35" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5" s="37">
+        <v>1</v>
+      </c>
+      <c r="D5" s="35" t="s">
+        <v>980</v>
+      </c>
+      <c r="E5" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="F5" s="38"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" s="37">
+        <v>1</v>
+      </c>
+      <c r="D6" s="35" t="s">
+        <v>980</v>
+      </c>
+      <c r="E6" s="35" t="s">
+        <v>980</v>
+      </c>
+      <c r="F6" s="35" t="s">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" s="39">
+        <v>2</v>
+      </c>
+      <c r="D7" s="35" t="s">
+        <v>982</v>
+      </c>
+      <c r="E7" s="35" t="s">
+        <v>976</v>
+      </c>
+      <c r="F7" s="35" t="s">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="C8" s="39">
+        <v>2</v>
+      </c>
+      <c r="D8" s="35" t="s">
+        <v>982</v>
+      </c>
+      <c r="E8" s="35" t="s">
+        <v>976</v>
+      </c>
+      <c r="F8" s="38"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" s="40">
+        <v>3</v>
+      </c>
+      <c r="D9" s="35" t="s">
+        <v>976</v>
+      </c>
+      <c r="E9" s="35" t="s">
+        <v>976</v>
+      </c>
+      <c r="F9" s="35" t="s">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" s="39">
+        <v>2</v>
+      </c>
+      <c r="D10" s="35" t="s">
+        <v>980</v>
+      </c>
+      <c r="E10" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="F10" s="35" t="s">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="35" t="s">
+        <v>106</v>
+      </c>
+      <c r="C11" s="37">
+        <v>1</v>
+      </c>
+      <c r="D11" s="35" t="s">
+        <v>982</v>
+      </c>
+      <c r="E11" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="F11" s="38"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="35" t="s">
+        <v>112</v>
+      </c>
+      <c r="C12" s="39">
+        <v>2</v>
+      </c>
+      <c r="D12" s="35" t="s">
+        <v>982</v>
+      </c>
+      <c r="E12" s="35" t="s">
+        <v>976</v>
+      </c>
+      <c r="F12" s="38"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="35" t="s">
+        <v>95</v>
+      </c>
+      <c r="C13" s="37">
+        <v>1</v>
+      </c>
+      <c r="D13" s="35" t="s">
+        <v>980</v>
+      </c>
+      <c r="E13" s="35" t="s">
+        <v>976</v>
+      </c>
+      <c r="F13" s="35" t="s">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="C14" s="37">
+        <v>1</v>
+      </c>
+      <c r="D14" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="E14" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="F14" s="38"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="35" t="s">
+        <v>113</v>
+      </c>
+      <c r="C15" s="39">
+        <v>2</v>
+      </c>
+      <c r="D15" s="35" t="s">
+        <v>980</v>
+      </c>
+      <c r="E15" s="35" t="s">
+        <v>980</v>
+      </c>
+      <c r="F15" s="35" t="s">
+        <v>986</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="35" t="s">
+        <v>114</v>
+      </c>
+      <c r="C16" s="37">
+        <v>1</v>
+      </c>
+      <c r="D16" s="35" t="s">
+        <v>982</v>
+      </c>
+      <c r="E16" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="F16" s="38"/>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="35" t="s">
+        <v>121</v>
+      </c>
+      <c r="C17" s="37">
+        <v>1</v>
+      </c>
+      <c r="D17" s="35" t="s">
+        <v>978</v>
+      </c>
+      <c r="E17" s="35" t="s">
+        <v>976</v>
+      </c>
+      <c r="F17" s="38"/>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="35" t="s">
+        <v>122</v>
+      </c>
+      <c r="C18" s="42">
+        <v>5</v>
+      </c>
+      <c r="D18" s="35" t="s">
+        <v>982</v>
+      </c>
+      <c r="E18" s="35" t="s">
+        <v>976</v>
+      </c>
+      <c r="F18" s="35" t="s">
+        <v>987</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="C19" s="43">
+        <v>4</v>
+      </c>
+      <c r="D19" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="E19" s="35" t="s">
+        <v>978</v>
+      </c>
+      <c r="F19" s="35" t="s">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="35" t="s">
+        <v>112</v>
+      </c>
+      <c r="C20" s="43">
+        <v>4</v>
+      </c>
+      <c r="D20" s="35" t="s">
+        <v>982</v>
+      </c>
+      <c r="E20" s="35" t="s">
+        <v>976</v>
+      </c>
+      <c r="F20" s="35" t="s">
+        <v>989</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="35" t="s">
+        <v>129</v>
+      </c>
+      <c r="C21" s="40">
+        <v>3</v>
+      </c>
+      <c r="D21" s="35" t="s">
+        <v>982</v>
+      </c>
+      <c r="E21" s="35" t="s">
+        <v>980</v>
+      </c>
+      <c r="F21" s="35" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="35" t="s">
+        <v>130</v>
+      </c>
+      <c r="C22" s="37">
+        <v>1</v>
+      </c>
+      <c r="D22" s="35" t="s">
+        <v>982</v>
+      </c>
+      <c r="E22" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="F22" s="38"/>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" s="35" t="s">
+        <v>134</v>
+      </c>
+      <c r="C23" s="43">
+        <v>4</v>
+      </c>
+      <c r="D23" s="35" t="s">
+        <v>976</v>
+      </c>
+      <c r="E23" s="35" t="s">
+        <v>980</v>
+      </c>
+      <c r="F23" s="35" t="s">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" s="35" t="s">
+        <v>137</v>
+      </c>
+      <c r="C24" s="37">
+        <v>1</v>
+      </c>
+      <c r="D24" s="35" t="s">
+        <v>982</v>
+      </c>
+      <c r="E24" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="F24" s="38"/>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25" s="35" t="s">
+        <v>139</v>
+      </c>
+      <c r="C25" s="39">
+        <v>2</v>
+      </c>
+      <c r="D25" s="35" t="s">
+        <v>982</v>
+      </c>
+      <c r="E25" s="35" t="s">
+        <v>980</v>
+      </c>
+      <c r="F25" s="35" t="s">
+        <v>992</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26" s="35" t="s">
+        <v>140</v>
+      </c>
+      <c r="C26" s="39">
+        <v>2</v>
+      </c>
+      <c r="D26" s="35" t="s">
+        <v>982</v>
+      </c>
+      <c r="E26" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="F26" s="38"/>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27" s="35" t="s">
+        <v>142</v>
+      </c>
+      <c r="C27" s="37">
+        <v>1</v>
+      </c>
+      <c r="D27" s="35" t="s">
+        <v>982</v>
+      </c>
+      <c r="E27" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="F27" s="38"/>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="B28" s="35" t="s">
+        <v>144</v>
+      </c>
+      <c r="C28" s="39">
+        <v>2</v>
+      </c>
+      <c r="D28" s="35" t="s">
+        <v>982</v>
+      </c>
+      <c r="E28" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="F28" s="38"/>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="B29" s="35" t="s">
+        <v>146</v>
+      </c>
+      <c r="C29" s="40">
+        <v>3</v>
+      </c>
+      <c r="D29" s="35" t="s">
+        <v>982</v>
+      </c>
+      <c r="E29" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="F29" s="35" t="s">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="41" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30" s="35" t="s">
+        <v>147</v>
+      </c>
+      <c r="C30" s="37">
+        <v>1</v>
+      </c>
+      <c r="D30" s="35" t="s">
+        <v>982</v>
+      </c>
+      <c r="E30" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="F30" s="38"/>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="B31" s="35" t="s">
+        <v>148</v>
+      </c>
+      <c r="C31" s="39">
+        <v>2</v>
+      </c>
+      <c r="D31" s="35" t="s">
+        <v>982</v>
+      </c>
+      <c r="E31" s="35" t="s">
+        <v>980</v>
+      </c>
+      <c r="F31" s="35" t="s">
+        <v>994</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="B32" s="35" t="s">
+        <v>110</v>
+      </c>
+      <c r="C32" s="37">
+        <v>1</v>
+      </c>
+      <c r="D32" s="35" t="s">
+        <v>977</v>
+      </c>
+      <c r="E32" s="35" t="s">
+        <v>995</v>
+      </c>
+      <c r="F32" s="35" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33" s="35" t="s">
+        <v>151</v>
+      </c>
+      <c r="C33" s="37">
+        <v>1</v>
+      </c>
+      <c r="D33" s="35" t="s">
+        <v>980</v>
+      </c>
+      <c r="E33" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="F33" s="35" t="s">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="B34" s="35" t="s">
+        <v>107</v>
+      </c>
+      <c r="C34" s="39">
+        <v>2</v>
+      </c>
+      <c r="D34" s="35" t="s">
+        <v>976</v>
+      </c>
+      <c r="E34" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="F34" s="38"/>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="B35" s="35" t="s">
+        <v>167</v>
+      </c>
+      <c r="C35" s="39">
+        <v>2</v>
+      </c>
+      <c r="D35" s="35" t="s">
+        <v>977</v>
+      </c>
+      <c r="E35" s="35" t="s">
+        <v>976</v>
+      </c>
+      <c r="F35" s="35" t="s">
+        <v>998</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="B36" s="35" t="s">
+        <v>95</v>
+      </c>
+      <c r="C36" s="37">
+        <v>1</v>
+      </c>
+      <c r="D36" s="35" t="s">
+        <v>982</v>
+      </c>
+      <c r="E36" s="35" t="s">
+        <v>980</v>
+      </c>
+      <c r="F36" s="35" t="s">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="B37" s="35" t="s">
+        <v>170</v>
+      </c>
+      <c r="C37" s="43">
+        <v>4</v>
+      </c>
+      <c r="D37" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="E37" s="35" t="s">
+        <v>976</v>
+      </c>
+      <c r="F37" s="38"/>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="B38" s="35" t="s">
+        <v>186</v>
+      </c>
+      <c r="C38" s="39">
+        <v>2</v>
+      </c>
+      <c r="D38" s="35" t="s">
+        <v>976</v>
+      </c>
+      <c r="E38" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="F38" s="38"/>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="B39" s="35" t="s">
+        <v>176</v>
+      </c>
+      <c r="C39" s="37">
+        <v>1</v>
+      </c>
+      <c r="D39" s="35" t="s">
+        <v>977</v>
+      </c>
+      <c r="E39" s="35" t="s">
+        <v>995</v>
+      </c>
+      <c r="F39" s="35" t="s">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="B40" s="35" t="s">
+        <v>179</v>
+      </c>
+      <c r="C40" s="39">
+        <v>2</v>
+      </c>
+      <c r="D40" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="E40" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="F40" s="35" t="s">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="B41" s="35" t="s">
+        <v>189</v>
+      </c>
+      <c r="C41" s="37">
+        <v>1</v>
+      </c>
+      <c r="D41" s="35" t="s">
+        <v>976</v>
+      </c>
+      <c r="E41" s="35" t="s">
+        <v>976</v>
+      </c>
+      <c r="F41" s="38"/>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="B42" s="35" t="s">
+        <v>190</v>
+      </c>
+      <c r="C42" s="37">
+        <v>1</v>
+      </c>
+      <c r="D42" s="35" t="s">
+        <v>982</v>
+      </c>
+      <c r="E42" s="35" t="s">
+        <v>980</v>
+      </c>
+      <c r="F42" s="35" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="B43" s="35" t="s">
+        <v>95</v>
+      </c>
+      <c r="C43" s="37">
+        <v>1</v>
+      </c>
+      <c r="D43" s="35" t="s">
+        <v>982</v>
+      </c>
+      <c r="E43" s="35" t="s">
+        <v>980</v>
+      </c>
+      <c r="F43" s="35" t="s">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="B44" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="C44" s="37">
+        <v>1</v>
+      </c>
+      <c r="D44" s="35" t="s">
+        <v>982</v>
+      </c>
+      <c r="E44" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="F44" s="38"/>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="B45" s="35" t="s">
+        <v>193</v>
+      </c>
+      <c r="C45" s="37">
+        <v>1</v>
+      </c>
+      <c r="D45" s="35" t="s">
+        <v>982</v>
+      </c>
+      <c r="E45" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="F45" s="38"/>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="B46" s="35" t="s">
+        <v>200</v>
+      </c>
+      <c r="C46" s="37">
+        <v>1</v>
+      </c>
+      <c r="D46" s="35" t="s">
+        <v>982</v>
+      </c>
+      <c r="E46" s="35" t="s">
+        <v>976</v>
+      </c>
+      <c r="F46" s="35" t="s">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="B47" s="35" t="s">
+        <v>208</v>
+      </c>
+      <c r="C47" s="37">
+        <v>1</v>
+      </c>
+      <c r="D47" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="E47" s="35" t="s">
+        <v>995</v>
+      </c>
+      <c r="F47" s="35" t="s">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="B48" s="35" t="s">
+        <v>95</v>
+      </c>
+      <c r="C48" s="44">
+        <v>8</v>
+      </c>
+      <c r="D48" s="35" t="s">
+        <v>982</v>
+      </c>
+      <c r="E48" s="35" t="s">
+        <v>980</v>
+      </c>
+      <c r="F48" s="35" t="s">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="B49" s="35" t="s">
+        <v>155</v>
+      </c>
+      <c r="C49" s="42">
+        <v>5</v>
+      </c>
+      <c r="D49" s="35" t="s">
+        <v>982</v>
+      </c>
+      <c r="E49" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="F49" s="35" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="B50" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="C50" s="45">
+        <v>9</v>
+      </c>
+      <c r="D50" s="35" t="s">
+        <v>982</v>
+      </c>
+      <c r="E50" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="F50" s="35" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" s="41" t="s">
+        <v>30</v>
+      </c>
+      <c r="B51" s="35" t="s">
+        <v>209</v>
+      </c>
+      <c r="C51" s="39">
+        <v>2</v>
+      </c>
+      <c r="D51" s="35" t="s">
+        <v>982</v>
+      </c>
+      <c r="E51" s="35" t="s">
+        <v>976</v>
+      </c>
+      <c r="F51" s="35" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="B52" s="35" t="s">
+        <v>210</v>
+      </c>
+      <c r="C52" s="37">
+        <v>1</v>
+      </c>
+      <c r="D52" s="35" t="s">
+        <v>980</v>
+      </c>
+      <c r="E52" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="F52" s="35" t="s">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="B53" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C53" s="37">
+        <v>1</v>
+      </c>
+      <c r="D53" s="35" t="s">
+        <v>982</v>
+      </c>
+      <c r="E53" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="F53" s="38"/>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="B54" s="35" t="s">
+        <v>222</v>
+      </c>
+      <c r="C54" s="37">
+        <v>1</v>
+      </c>
+      <c r="D54" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="E54" s="35" t="s">
+        <v>980</v>
+      </c>
+      <c r="F54" s="35" t="s">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="B55" s="35" t="s">
+        <v>225</v>
+      </c>
+      <c r="C55" s="37">
+        <v>1</v>
+      </c>
+      <c r="D55" s="35" t="s">
+        <v>980</v>
+      </c>
+      <c r="E55" s="35" t="s">
+        <v>980</v>
+      </c>
+      <c r="F55" s="35" t="s">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="B56" s="35" t="s">
+        <v>228</v>
+      </c>
+      <c r="C56" s="37">
+        <v>1</v>
+      </c>
+      <c r="D56" s="35" t="s">
+        <v>980</v>
+      </c>
+      <c r="E56" s="35" t="s">
+        <v>980</v>
+      </c>
+      <c r="F56" s="35" t="s">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="B57" s="35" t="s">
+        <v>229</v>
+      </c>
+      <c r="C57" s="37">
+        <v>1</v>
+      </c>
+      <c r="D57" s="35" t="s">
+        <v>982</v>
+      </c>
+      <c r="E57" s="35" t="s">
+        <v>980</v>
+      </c>
+      <c r="F57" s="35" t="s">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="B58" s="35" t="s">
+        <v>237</v>
+      </c>
+      <c r="C58" s="37">
+        <v>1</v>
+      </c>
+      <c r="D58" s="35" t="s">
+        <v>982</v>
+      </c>
+      <c r="E58" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="F58" s="38"/>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="A59" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="B59" s="35" t="s">
+        <v>240</v>
+      </c>
+      <c r="C59" s="42">
+        <v>5</v>
+      </c>
+      <c r="D59" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="E59" s="35" t="s">
+        <v>980</v>
+      </c>
+      <c r="F59" s="35" t="s">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B60" s="35" t="s">
+        <v>241</v>
+      </c>
+      <c r="C60" s="37">
+        <v>1</v>
+      </c>
+      <c r="D60" s="35" t="s">
+        <v>980</v>
+      </c>
+      <c r="E60" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="F60" s="35" t="s">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="B61" s="35" t="s">
+        <v>242</v>
+      </c>
+      <c r="C61" s="37">
+        <v>1</v>
+      </c>
+      <c r="D61" s="35" t="s">
+        <v>982</v>
+      </c>
+      <c r="E61" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="F61" s="38"/>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="B62" s="35" t="s">
+        <v>243</v>
+      </c>
+      <c r="C62" s="37">
+        <v>1</v>
+      </c>
+      <c r="D62" s="35" t="s">
+        <v>982</v>
+      </c>
+      <c r="E62" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="F62" s="38"/>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="B63" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="C63" s="37">
+        <v>1</v>
+      </c>
+      <c r="D63" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="E63" s="35" t="s">
+        <v>976</v>
+      </c>
+      <c r="F63" s="38"/>
+    </row>
+    <row r="64" spans="1:6">
+      <c r="A64" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="B64" s="35" t="s">
+        <v>262</v>
+      </c>
+      <c r="C64" s="43">
+        <v>4</v>
+      </c>
+      <c r="D64" s="35" t="s">
+        <v>976</v>
+      </c>
+      <c r="E64" s="35" t="s">
+        <v>976</v>
+      </c>
+      <c r="F64" s="35" t="s">
+        <v>1017</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
+      <c r="A65" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="B65" s="35" t="s">
+        <v>263</v>
+      </c>
+      <c r="C65" s="40">
+        <v>3</v>
+      </c>
+      <c r="D65" s="35" t="s">
+        <v>982</v>
+      </c>
+      <c r="E65" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="F65" s="35" t="s">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="A66" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="B66" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="C66" s="37">
+        <v>1</v>
+      </c>
+      <c r="D66" s="35" t="s">
+        <v>982</v>
+      </c>
+      <c r="E66" s="35" t="s">
+        <v>976</v>
+      </c>
+      <c r="F66" s="38"/>
+    </row>
+    <row r="67" spans="1:6">
+      <c r="A67" s="41" t="s">
+        <v>36</v>
+      </c>
+      <c r="B67" s="35" t="s">
+        <v>265</v>
+      </c>
+      <c r="C67" s="39">
+        <v>2</v>
+      </c>
+      <c r="D67" s="35" t="s">
+        <v>982</v>
+      </c>
+      <c r="E67" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="F67" s="35" t="s">
+        <v>1019</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
+      <c r="A68" s="41" t="s">
+        <v>37</v>
+      </c>
+      <c r="B68" s="35" t="s">
+        <v>264</v>
+      </c>
+      <c r="C68" s="39">
+        <v>2</v>
+      </c>
+      <c r="D68" s="35" t="s">
+        <v>982</v>
+      </c>
+      <c r="E68" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="F68" s="38"/>
+    </row>
+    <row r="69" spans="1:6">
+      <c r="A69" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="B69" s="35" t="s">
+        <v>266</v>
+      </c>
+      <c r="C69" s="40">
+        <v>3</v>
+      </c>
+      <c r="D69" s="35" t="s">
+        <v>982</v>
+      </c>
+      <c r="E69" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="F69" s="35" t="s">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
+      <c r="A70" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="B70" s="35" t="s">
+        <v>180</v>
+      </c>
+      <c r="C70" s="37">
+        <v>1</v>
+      </c>
+      <c r="D70" s="35" t="s">
+        <v>976</v>
+      </c>
+      <c r="E70" s="35" t="s">
+        <v>980</v>
+      </c>
+      <c r="F70" s="35" t="s">
+        <v>1021</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6">
+      <c r="A71" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="B71" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="C71" s="37">
+        <v>1</v>
+      </c>
+      <c r="D71" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="E71" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="F71" s="38"/>
+    </row>
+    <row r="72" spans="1:6">
+      <c r="A72" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="B72" s="35" t="s">
+        <v>271</v>
+      </c>
+      <c r="C72" s="40">
+        <v>3</v>
+      </c>
+      <c r="D72" s="35" t="s">
+        <v>982</v>
+      </c>
+      <c r="E72" s="35" t="s">
+        <v>980</v>
+      </c>
+      <c r="F72" s="35" t="s">
+        <v>1022</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6">
+      <c r="A73" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="B73" s="35" t="s">
+        <v>272</v>
+      </c>
+      <c r="C73" s="42">
+        <v>5</v>
+      </c>
+      <c r="D73" s="35" t="s">
+        <v>980</v>
+      </c>
+      <c r="E73" s="35" t="s">
+        <v>976</v>
+      </c>
+      <c r="F73" s="35" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6">
+      <c r="A74" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="B74" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C74" s="39">
+        <v>2</v>
+      </c>
+      <c r="D74" s="35" t="s">
+        <v>980</v>
+      </c>
+      <c r="E74" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="F74" s="35" t="s">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6">
+      <c r="A75" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="B75" s="35" t="s">
+        <v>146</v>
+      </c>
+      <c r="C75" s="37">
+        <v>1</v>
+      </c>
+      <c r="D75" s="35" t="s">
+        <v>980</v>
+      </c>
+      <c r="E75" s="35" t="s">
+        <v>978</v>
+      </c>
+      <c r="F75" s="35" t="s">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6">
+      <c r="A76" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="B76" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="C76" s="39">
+        <v>2</v>
+      </c>
+      <c r="D76" s="35" t="s">
+        <v>982</v>
+      </c>
+      <c r="E76" s="35" t="s">
+        <v>976</v>
+      </c>
+      <c r="F76" s="38"/>
+    </row>
+    <row r="77" spans="1:6">
+      <c r="A77" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="B77" s="35" t="s">
+        <v>277</v>
+      </c>
+      <c r="C77" s="40">
+        <v>3</v>
+      </c>
+      <c r="D77" s="35" t="s">
+        <v>982</v>
+      </c>
+      <c r="E77" s="35" t="s">
+        <v>980</v>
+      </c>
+      <c r="F77" s="35" t="s">
+        <v>1026</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6">
+      <c r="A78" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="B78" s="35" t="s">
+        <v>278</v>
+      </c>
+      <c r="C78" s="37">
+        <v>1</v>
+      </c>
+      <c r="D78" s="35" t="s">
+        <v>978</v>
+      </c>
+      <c r="E78" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="F78" s="38"/>
+    </row>
+    <row r="79" spans="1:6">
+      <c r="A79" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="B79" s="35" t="s">
+        <v>279</v>
+      </c>
+      <c r="C79" s="37">
+        <v>1</v>
+      </c>
+      <c r="D79" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="E79" s="35" t="s">
+        <v>976</v>
+      </c>
+      <c r="F79" s="38"/>
+    </row>
+    <row r="80" spans="1:6">
+      <c r="A80" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="B80" s="35" t="s">
+        <v>280</v>
+      </c>
+      <c r="C80" s="37">
+        <v>1</v>
+      </c>
+      <c r="D80" s="35" t="s">
+        <v>982</v>
+      </c>
+      <c r="E80" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="F80" s="38"/>
+    </row>
+    <row r="81" spans="1:6">
+      <c r="A81" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="B81" s="35" t="s">
+        <v>281</v>
+      </c>
+      <c r="C81" s="37">
+        <v>1</v>
+      </c>
+      <c r="D81" s="35" t="s">
+        <v>982</v>
+      </c>
+      <c r="E81" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="F81" s="38"/>
+    </row>
+    <row r="82" spans="1:6">
+      <c r="A82" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="B82" s="35" t="s">
+        <v>144</v>
+      </c>
+      <c r="C82" s="43">
+        <v>4</v>
+      </c>
+      <c r="D82" s="35" t="s">
+        <v>982</v>
+      </c>
+      <c r="E82" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="F82" s="38"/>
+    </row>
+    <row r="83" spans="1:6">
+      <c r="A83" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="B83" s="35" t="s">
+        <v>95</v>
+      </c>
+      <c r="C83" s="39">
+        <v>2</v>
+      </c>
+      <c r="D83" s="35" t="s">
+        <v>976</v>
+      </c>
+      <c r="E83" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="F83" s="35" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6">
+      <c r="A84" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="B84" s="35" t="s">
+        <v>289</v>
+      </c>
+      <c r="C84" s="39">
+        <v>2</v>
+      </c>
+      <c r="D84" s="35" t="s">
+        <v>976</v>
+      </c>
+      <c r="E84" s="35" t="s">
+        <v>976</v>
+      </c>
+      <c r="F84" s="38"/>
+    </row>
+    <row r="85" spans="1:6">
+      <c r="A85" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="B85" s="35" t="s">
+        <v>291</v>
+      </c>
+      <c r="C85" s="39">
+        <v>2</v>
+      </c>
+      <c r="D85" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="E85" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="F85" s="38"/>
+    </row>
+    <row r="86" spans="1:6">
+      <c r="A86" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="B86" s="35" t="s">
+        <v>298</v>
+      </c>
+      <c r="C86" s="37">
+        <v>1</v>
+      </c>
+      <c r="D86" s="35" t="s">
+        <v>982</v>
+      </c>
+      <c r="E86" s="35" t="s">
+        <v>995</v>
+      </c>
+      <c r="F86" s="35" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6">
+      <c r="A87" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="B87" s="35" t="s">
+        <v>330</v>
+      </c>
+      <c r="C87" s="37">
+        <v>1</v>
+      </c>
+      <c r="D87" s="35" t="s">
+        <v>982</v>
+      </c>
+      <c r="E87" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="F87" s="38"/>
+    </row>
+    <row r="88" spans="1:6">
+      <c r="A88" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="B88" s="35" t="s">
+        <v>331</v>
+      </c>
+      <c r="C88" s="39">
+        <v>2</v>
+      </c>
+      <c r="D88" s="35" t="s">
+        <v>982</v>
+      </c>
+      <c r="E88" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="F88" s="38"/>
+    </row>
+    <row r="89" spans="1:6">
+      <c r="A89" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="B89" s="35" t="s">
+        <v>332</v>
+      </c>
+      <c r="C89" s="37">
+        <v>1</v>
+      </c>
+      <c r="D89" s="35" t="s">
+        <v>982</v>
+      </c>
+      <c r="E89" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="F89" s="38"/>
+    </row>
+    <row r="90" spans="1:6">
+      <c r="A90" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="B90" s="35" t="s">
+        <v>163</v>
+      </c>
+      <c r="C90" s="37">
+        <v>1</v>
+      </c>
+      <c r="D90" s="35" t="s">
+        <v>980</v>
+      </c>
+      <c r="E90" s="35" t="s">
+        <v>980</v>
+      </c>
+      <c r="F90" s="35" t="s">
+        <v>1029</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6">
+      <c r="A91" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="B91" s="35" t="s">
+        <v>364</v>
+      </c>
+      <c r="C91" s="37">
+        <v>1</v>
+      </c>
+      <c r="D91" s="35" t="s">
+        <v>980</v>
+      </c>
+      <c r="E91" s="35" t="s">
+        <v>976</v>
+      </c>
+      <c r="F91" s="35" t="s">
+        <v>1030</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6">
+      <c r="A92" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="B92" s="35" t="s">
+        <v>369</v>
+      </c>
+      <c r="C92" s="37">
+        <v>1</v>
+      </c>
+      <c r="D92" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="E92" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="F92" s="38"/>
+    </row>
+    <row r="93" spans="1:6">
+      <c r="A93" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="B93" s="35" t="s">
+        <v>373</v>
+      </c>
+      <c r="C93" s="39">
+        <v>2</v>
+      </c>
+      <c r="D93" s="35" t="s">
+        <v>982</v>
+      </c>
+      <c r="E93" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="F93" s="38"/>
+    </row>
+    <row r="94" spans="1:6">
+      <c r="A94" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="B94" s="35" t="s">
+        <v>398</v>
+      </c>
+      <c r="C94" s="37">
+        <v>1</v>
+      </c>
+      <c r="D94" s="35" t="s">
+        <v>982</v>
+      </c>
+      <c r="E94" s="35" t="s">
+        <v>980</v>
+      </c>
+      <c r="F94" s="35" t="s">
+        <v>1031</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6">
+      <c r="A95" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="B95" s="35" t="s">
+        <v>411</v>
+      </c>
+      <c r="C95" s="42">
+        <v>5</v>
+      </c>
+      <c r="D95" s="35" t="s">
+        <v>976</v>
+      </c>
+      <c r="E95" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="F95" s="35" t="s">
+        <v>1032</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6">
+      <c r="A96" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="B96" s="35" t="s">
+        <v>144</v>
+      </c>
+      <c r="C96" s="46">
+        <v>12</v>
+      </c>
+      <c r="D96" s="35" t="s">
+        <v>982</v>
+      </c>
+      <c r="E96" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="F96" s="35" t="s">
+        <v>1033</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6">
+      <c r="A97" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="B97" s="35" t="s">
+        <v>165</v>
+      </c>
+      <c r="C97" s="43">
+        <v>4</v>
+      </c>
+      <c r="D97" s="35" t="s">
+        <v>982</v>
+      </c>
+      <c r="E97" s="35" t="s">
+        <v>976</v>
+      </c>
+      <c r="F97" s="35" t="s">
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6">
+      <c r="A98" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="B98" s="35" t="s">
+        <v>424</v>
+      </c>
+      <c r="C98" s="43">
+        <v>4</v>
+      </c>
+      <c r="D98" s="35" t="s">
+        <v>978</v>
+      </c>
+      <c r="E98" s="35" t="s">
+        <v>980</v>
+      </c>
+      <c r="F98" s="35" t="s">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6">
+      <c r="A99" s="41" t="s">
+        <v>52</v>
+      </c>
+      <c r="B99" s="35" t="s">
+        <v>147</v>
+      </c>
+      <c r="C99" s="42">
+        <v>5</v>
+      </c>
+      <c r="D99" s="35" t="s">
+        <v>982</v>
+      </c>
+      <c r="E99" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="F99" s="35" t="s">
+        <v>1036</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6">
+      <c r="A100" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="B100" s="35" t="s">
+        <v>425</v>
+      </c>
+      <c r="C100" s="39">
+        <v>2</v>
+      </c>
+      <c r="D100" s="35" t="s">
+        <v>982</v>
+      </c>
+      <c r="E100" s="35" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F100" s="38"/>
+    </row>
+    <row r="101" spans="1:6">
+      <c r="A101" s="36" t="s">
+        <v>54</v>
+      </c>
+      <c r="B101" s="35" t="s">
+        <v>331</v>
+      </c>
+      <c r="C101" s="37">
+        <v>1</v>
+      </c>
+      <c r="D101" s="35" t="s">
+        <v>982</v>
+      </c>
+      <c r="E101" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="F101" s="38"/>
+    </row>
+    <row r="102" spans="1:6">
+      <c r="A102" s="36" t="s">
+        <v>54</v>
+      </c>
+      <c r="B102" s="35" t="s">
+        <v>441</v>
+      </c>
+      <c r="C102" s="37">
+        <v>1</v>
+      </c>
+      <c r="D102" s="35" t="s">
+        <v>980</v>
+      </c>
+      <c r="E102" s="35" t="s">
+        <v>980</v>
+      </c>
+      <c r="F102" s="35" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6">
+      <c r="A103" s="36" t="s">
+        <v>54</v>
+      </c>
+      <c r="B103" s="35" t="s">
+        <v>448</v>
+      </c>
+      <c r="C103" s="37">
+        <v>1</v>
+      </c>
+      <c r="D103" s="35" t="s">
+        <v>976</v>
+      </c>
+      <c r="E103" s="35" t="s">
+        <v>978</v>
+      </c>
+      <c r="F103" s="38"/>
+    </row>
+    <row r="104" spans="1:6">
+      <c r="A104" s="36" t="s">
+        <v>54</v>
+      </c>
+      <c r="B104" s="35" t="s">
+        <v>449</v>
+      </c>
+      <c r="C104" s="37">
+        <v>1</v>
+      </c>
+      <c r="D104" s="35" t="s">
+        <v>982</v>
+      </c>
+      <c r="E104" s="35" t="s">
+        <v>976</v>
+      </c>
+      <c r="F104" s="38"/>
+    </row>
+    <row r="105" spans="1:6">
+      <c r="A105" s="36" t="s">
+        <v>54</v>
+      </c>
+      <c r="B105" s="35" t="s">
+        <v>450</v>
+      </c>
+      <c r="C105" s="37">
+        <v>1</v>
+      </c>
+      <c r="D105" s="35" t="s">
+        <v>982</v>
+      </c>
+      <c r="E105" s="35" t="s">
+        <v>978</v>
+      </c>
+      <c r="F105" s="38"/>
+    </row>
+    <row r="106" spans="1:6">
+      <c r="A106" s="36" t="s">
+        <v>54</v>
+      </c>
+      <c r="B106" s="35" t="s">
+        <v>454</v>
+      </c>
+      <c r="C106" s="37">
+        <v>1</v>
+      </c>
+      <c r="D106" s="35" t="s">
+        <v>982</v>
+      </c>
+      <c r="E106" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="F106" s="38"/>
+    </row>
+    <row r="107" spans="1:6">
+      <c r="A107" s="36" t="s">
+        <v>54</v>
+      </c>
+      <c r="B107" s="35" t="s">
+        <v>463</v>
+      </c>
+      <c r="C107" s="37">
+        <v>1</v>
+      </c>
+      <c r="D107" s="35" t="s">
+        <v>982</v>
+      </c>
+      <c r="E107" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="F107" s="38"/>
+    </row>
+    <row r="108" spans="1:6">
+      <c r="A108" s="41" t="s">
+        <v>54</v>
+      </c>
+      <c r="B108" s="35" t="s">
+        <v>465</v>
+      </c>
+      <c r="C108" s="37">
+        <v>1</v>
+      </c>
+      <c r="D108" s="35" t="s">
+        <v>982</v>
+      </c>
+      <c r="E108" s="35" t="s">
+        <v>976</v>
+      </c>
+      <c r="F108" s="38"/>
+    </row>
+    <row r="109" spans="1:6">
+      <c r="A109" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="B109" s="35" t="s">
+        <v>466</v>
+      </c>
+      <c r="C109" s="40">
+        <v>3</v>
+      </c>
+      <c r="D109" s="35" t="s">
+        <v>982</v>
+      </c>
+      <c r="E109" s="35" t="s">
+        <v>979</v>
+      </c>
+      <c r="F109" s="38"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>